<commit_message>
State machine and alarm updates
</commit_message>
<xml_diff>
--- a/Documentation/Software/Input-Ouput_Details.xlsx
+++ b/Documentation/Software/Input-Ouput_Details.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
   <si>
     <t>Connections</t>
   </si>
@@ -237,6 +237,33 @@
   </si>
   <si>
     <t>TX</t>
+  </si>
+  <si>
+    <t>20 (SDA)</t>
+  </si>
+  <si>
+    <t>21 (SCL)</t>
+  </si>
+  <si>
+    <t>17 (RX2)</t>
+  </si>
+  <si>
+    <t>16 (TX2)</t>
+  </si>
+  <si>
+    <t>Outputs</t>
+  </si>
+  <si>
+    <t>Alarm Buzzer</t>
+  </si>
+  <si>
+    <t>Alarm LCD</t>
+  </si>
+  <si>
+    <t>Alarm Relay</t>
+  </si>
+  <si>
+    <t>Digital Output</t>
   </si>
 </sst>
 </file>
@@ -276,7 +303,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,6 +352,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -425,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -438,16 +471,38 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -456,33 +511,34 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -764,11 +820,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,199 +849,231 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="9"/>
       <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="26">
+        <v>4</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>55</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="26">
+        <v>5</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="26">
+        <v>6</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="26">
+        <v>7</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="26">
+        <v>8</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="14" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="26">
+        <v>9</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="26">
+        <v>22</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="26">
+        <v>24</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="26">
+        <v>26</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="26">
+        <v>28</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="26">
+        <v>30</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="26">
+        <v>32</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="14" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="26">
+        <v>34</v>
+      </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="26">
+        <v>36</v>
+      </c>
       <c r="D16" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>52</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="27">
+        <v>10</v>
+      </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="27">
+        <v>18</v>
+      </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -993,7 +1081,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="16"/>
-      <c r="C19" s="10"/>
+      <c r="C19" s="13"/>
       <c r="D19" s="8"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1003,7 +1091,9 @@
       <c r="B20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="27">
+        <v>2</v>
+      </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1013,7 +1103,9 @@
       <c r="B21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="27">
+        <v>3</v>
+      </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1023,7 +1115,9 @@
       <c r="B22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="27">
+        <v>19</v>
+      </c>
       <c r="D22" s="2" t="s">
         <v>30</v>
       </c>
@@ -1033,7 +1127,7 @@
         <v>31</v>
       </c>
       <c r="B23" s="16"/>
-      <c r="C23" s="5"/>
+      <c r="C23" s="13"/>
       <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1043,117 +1137,143 @@
       <c r="B24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="26">
+        <v>38</v>
+      </c>
       <c r="D24" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="1"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="28"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="26">
+        <v>53</v>
+      </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="26">
+        <v>51</v>
+      </c>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="3"/>
+      <c r="C28" s="26">
+        <v>47</v>
+      </c>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="3"/>
+      <c r="C29" s="26">
+        <v>45</v>
+      </c>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="3"/>
+      <c r="C30" s="26">
+        <v>43</v>
+      </c>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="3"/>
+      <c r="C31" s="26">
+        <v>41</v>
+      </c>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="3"/>
+      <c r="C32" s="26">
+        <v>53</v>
+      </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="3"/>
+      <c r="C33" s="26">
+        <v>49</v>
+      </c>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="3"/>
+      <c r="C34" s="26">
+        <v>47</v>
+      </c>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="3"/>
+      <c r="C35" s="26">
+        <v>45</v>
+      </c>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="3"/>
+      <c r="C36" s="26">
+        <v>43</v>
+      </c>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="3"/>
+      <c r="C37" s="26">
+        <v>41</v>
+      </c>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1161,65 +1281,118 @@
         <v>53</v>
       </c>
       <c r="B38" s="16"/>
-      <c r="C38" s="8"/>
+      <c r="C38" s="29"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C39" s="23"/>
+      <c r="C39" s="30" t="s">
+        <v>71</v>
+      </c>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="23" t="s">
+      <c r="A40" s="18"/>
+      <c r="B40" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C40" s="23"/>
+      <c r="C40" s="30" t="s">
+        <v>72</v>
+      </c>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="22"/>
-      <c r="C41" s="1"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="28"/>
       <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="23"/>
+      <c r="C42" s="30" t="s">
+        <v>73</v>
+      </c>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="20"/>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="23"/>
+      <c r="C43" s="30" t="s">
+        <v>74</v>
+      </c>
       <c r="D43" s="2"/>
     </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="31"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="34">
+        <v>11</v>
+      </c>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="34">
+        <v>12</v>
+      </c>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" s="34">
+        <v>13</v>
+      </c>
+      <c r="D47" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A32:A37"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>